<commit_message>
Remove redundant file, fix references
</commit_message>
<xml_diff>
--- a/pwm/ugv/tables/components.xlsx
+++ b/pwm/ugv/tables/components.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\goats\Documents\ssconvert\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A74A31C8-BD0A-466A-AB9C-4020C1B5B6B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94AE6848-E607-4722-90B3-A4A19F19591F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="16220" xr2:uid="{7E177AAD-D9CF-4325-9FA3-34BB7ACA35DC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Component</t>
   </si>
@@ -75,6 +75,9 @@
   </si>
   <si>
     <t>12 V</t>
+  </si>
+  <si>
+    <t>UGV Kit</t>
   </si>
 </sst>
 </file>
@@ -459,10 +462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A462B94-B289-4397-9ED0-7986D145C6DA}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -534,13 +537,22 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="4">
         <v>1</v>
       </c>
     </row>

</xml_diff>